<commit_message>
editing saving method for cart
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -1,78 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie\PycharmProjects\pythonProject1\AppDev\website\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE322110-5F24-4BB7-884C-CBB2EA87B651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5565" windowWidth="38640" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8910" yWindow="5565" windowWidth="38640" windowHeight="15435" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="damien" sheetId="2" r:id="rId1"/>
+    <sheet name="damien" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Measurement</t>
-  </si>
-  <si>
-    <t>Ingredient</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Canned Tomatoes</t>
-  </si>
-  <si>
-    <t>Dried Pasta</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Tablespoon Vegetable Oil</t>
-  </si>
-  <si>
-    <t>Grated Cheese</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -91,22 +51,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -394,82 +413,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Measurement</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>400</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>0.5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6">
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>200</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Canned Tomatoes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>75</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dried Pasta</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tablespoon Vegetable Oil</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Grated Cheese</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>200</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Canned Tomatoes</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>75</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dried Pasta</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Tablespoon Vegetable Oil</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>20</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Grated Cheese</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cart edit part 2
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
@@ -62,7 +62,9 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,12 +108,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,15 +481,15 @@
   </sheetPr>
   <dimension ref="A1:BS32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BT14" sqref="BT14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="16.140625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.28515625" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9.42578125" customWidth="1" min="22" max="22"/>
+    <col width="16.1796875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.26953125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9.453125" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -513,7 +515,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Garlic Clove</t>
+          <t>Garlic Cloves</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -843,7 +845,7 @@
       </c>
       <c r="BS1" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>Water</t>
         </is>
       </c>
     </row>
@@ -1070,214 +1072,214 @@
           <t>Price</t>
         </is>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="11" t="n">
         <v>2.85</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="11" t="n">
         <v>2.14</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="11" t="n">
         <v>2.42</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E3" s="11" t="n">
         <v>1.8</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="11" t="n">
         <v>3.97</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="11" t="n">
         <v>1.82</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="11" t="n">
         <v>5.5</v>
       </c>
-      <c r="I3" s="10" t="n">
+      <c r="I3" s="11" t="n">
         <v>0.96</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="11" t="n">
         <v>2.98</v>
       </c>
-      <c r="K3" s="10" t="n">
+      <c r="K3" s="11" t="n">
         <v>1.21</v>
       </c>
-      <c r="L3" s="10" t="n">
+      <c r="L3" s="11" t="n">
         <v>1.52</v>
       </c>
-      <c r="M3" s="10" t="n">
+      <c r="M3" s="11" t="n">
         <v>2.11</v>
       </c>
-      <c r="N3" s="10" t="n">
+      <c r="N3" s="11" t="n">
         <v>6.72</v>
       </c>
-      <c r="O3" s="10" t="n">
+      <c r="O3" s="11" t="n">
         <v>1.98</v>
       </c>
-      <c r="P3" s="10" t="n">
+      <c r="P3" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q3" s="10" t="n">
+      <c r="Q3" s="11" t="n">
         <v>8.5</v>
       </c>
-      <c r="R3" s="10" t="n">
+      <c r="R3" s="11" t="n">
         <v>6.45</v>
       </c>
-      <c r="S3" s="10" t="n">
+      <c r="S3" s="11" t="n">
         <v>2.21</v>
       </c>
-      <c r="T3" s="10" t="n">
+      <c r="T3" s="11" t="n">
         <v>5.85</v>
       </c>
-      <c r="U3" s="10" t="n">
+      <c r="U3" s="11" t="n">
         <v>0.46</v>
       </c>
-      <c r="V3" s="10" t="n">
+      <c r="V3" s="11" t="n">
         <v>5.95</v>
       </c>
-      <c r="W3" s="10" t="n">
+      <c r="W3" s="11" t="n">
         <v>3.82</v>
       </c>
-      <c r="X3" s="10" t="n">
+      <c r="X3" s="11" t="n">
         <v>2.98</v>
       </c>
-      <c r="Y3" s="10" t="n">
+      <c r="Y3" s="11" t="n">
         <v>4.8</v>
       </c>
-      <c r="Z3" s="10" t="n">
+      <c r="Z3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="AA3" s="10" t="n">
+      <c r="AA3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="AB3" s="10" t="n">
+      <c r="AB3" s="11" t="n">
         <v>3.75</v>
       </c>
-      <c r="AC3" s="10" t="n">
+      <c r="AC3" s="11" t="n">
         <v>1.8</v>
       </c>
-      <c r="AD3" s="10" t="n">
+      <c r="AD3" s="11" t="n">
         <v>2.22</v>
       </c>
-      <c r="AE3" s="10" t="n">
+      <c r="AE3" s="11" t="n">
         <v>9.85</v>
       </c>
-      <c r="AF3" s="10" t="n">
+      <c r="AF3" s="11" t="n">
         <v>1.99</v>
       </c>
-      <c r="AG3" s="10" t="n">
+      <c r="AG3" s="11" t="n">
         <v>1.37</v>
       </c>
-      <c r="AH3" s="10" t="n">
+      <c r="AH3" s="11" t="n">
         <v>1.12</v>
       </c>
-      <c r="AI3" s="10" t="n">
+      <c r="AI3" s="11" t="n">
         <v>1.62</v>
       </c>
-      <c r="AJ3" s="10" t="n">
+      <c r="AJ3" s="11" t="n">
         <v>0.86</v>
       </c>
-      <c r="AK3" s="10" t="n">
+      <c r="AK3" s="11" t="n">
         <v>3.65</v>
       </c>
-      <c r="AL3" s="10" t="n">
+      <c r="AL3" s="11" t="n">
         <v>3.17</v>
       </c>
-      <c r="AM3" s="10" t="n">
+      <c r="AM3" s="11" t="n">
         <v>5.98</v>
       </c>
-      <c r="AN3" s="10" t="n">
+      <c r="AN3" s="11" t="n">
         <v>4.19</v>
       </c>
-      <c r="AO3" s="10" t="n">
+      <c r="AO3" s="11" t="n">
         <v>5.66</v>
       </c>
-      <c r="AP3" s="10" t="n">
+      <c r="AP3" s="11" t="n">
         <v>3.14</v>
       </c>
-      <c r="AQ3" s="10" t="n">
+      <c r="AQ3" s="11" t="n">
         <v>7.95</v>
       </c>
-      <c r="AR3" s="10" t="n">
+      <c r="AR3" s="11" t="n">
         <v>4.5</v>
       </c>
-      <c r="AS3" s="10" t="n">
+      <c r="AS3" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="AT3" s="10" t="n">
+      <c r="AT3" s="11" t="n">
         <v>7.9</v>
       </c>
-      <c r="AU3" s="10" t="n">
+      <c r="AU3" s="11" t="n">
         <v>4.34</v>
       </c>
-      <c r="AV3" s="10" t="n">
+      <c r="AV3" s="11" t="n">
         <v>3.85</v>
       </c>
-      <c r="AW3" s="10" t="n">
+      <c r="AW3" s="11" t="n">
         <v>0.14</v>
       </c>
-      <c r="AX3" s="10" t="n">
+      <c r="AX3" s="11" t="n">
         <v>3.7</v>
       </c>
-      <c r="AY3" s="10" t="n">
+      <c r="AY3" s="11" t="n">
         <v>2.32</v>
       </c>
-      <c r="AZ3" s="10" t="n">
+      <c r="AZ3" s="11" t="n">
         <v>1.98</v>
       </c>
-      <c r="BA3" s="10" t="n">
+      <c r="BA3" s="11" t="n">
         <v>3.02</v>
       </c>
-      <c r="BB3" s="10" t="n">
+      <c r="BB3" s="11" t="n">
         <v>6.5</v>
       </c>
-      <c r="BC3" s="10" t="n">
+      <c r="BC3" s="11" t="n">
         <v>1.4</v>
       </c>
-      <c r="BD3" s="10" t="n">
+      <c r="BD3" s="11" t="n">
         <v>3.95</v>
       </c>
-      <c r="BE3" s="10" t="n">
+      <c r="BE3" s="11" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="BF3" s="10" t="n">
+      <c r="BF3" s="11" t="n">
         <v>9.9</v>
       </c>
-      <c r="BG3" s="10" t="n">
+      <c r="BG3" s="11" t="n">
         <v>1.38</v>
       </c>
-      <c r="BH3" s="10" t="n">
+      <c r="BH3" s="11" t="n">
         <v>1.15</v>
       </c>
-      <c r="BI3" s="10" t="n">
+      <c r="BI3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="BJ3" s="10" t="n">
+      <c r="BJ3" s="11" t="n">
         <v>11.91</v>
       </c>
-      <c r="BK3" s="10" t="n">
+      <c r="BK3" s="11" t="n">
         <v>5.98</v>
       </c>
-      <c r="BL3" s="10" t="n">
+      <c r="BL3" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="BM3" s="10" t="n">
+      <c r="BM3" s="11" t="n">
         <v>2.55</v>
       </c>
-      <c r="BN3" s="10" t="n">
+      <c r="BN3" s="11" t="n">
         <v>7.65</v>
       </c>
-      <c r="BO3" s="10" t="n">
+      <c r="BO3" s="11" t="n">
         <v>1.61</v>
       </c>
-      <c r="BP3" s="10" t="n">
+      <c r="BP3" s="11" t="n">
         <v>2.14</v>
       </c>
-      <c r="BQ3" s="10" t="n">
+      <c r="BQ3" s="11" t="n">
         <v>1.8</v>
       </c>
-      <c r="BR3" s="10" t="n">
+      <c r="BR3" s="11" t="n">
         <v>2.22</v>
       </c>
-      <c r="BS3" s="11" t="n">
+      <c r="BS3" s="12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1294,7 +1296,7 @@
       <c r="AY7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="n"/>
+      <c r="A8" s="13" t="n"/>
       <c r="AY8" s="2" t="n"/>
     </row>
     <row r="9">
@@ -1389,13 +1391,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="inlineStr">
@@ -1423,7 +1425,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Carrot</t>
+          <t>Capsicum</t>
         </is>
       </c>
     </row>
@@ -1432,11 +1434,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Capsicum</t>
+          <t>Garlic Cloves</t>
         </is>
       </c>
     </row>
@@ -1445,24 +1447,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.5</v>
+        <v>29.58</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Garlic Cloves</t>
+          <t>Chicken Stock</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>29.58</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Chicken Stock</t>
+          <t>Garlic Cloves</t>
         </is>
       </c>
     </row>
@@ -1471,11 +1473,11 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Pinch Sugar</t>
         </is>
       </c>
     </row>
@@ -1484,35 +1486,9 @@
         <v>4</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C7" t="inlineStr">
-        <is>
-          <t>Garlic Cloves</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Pinch Sugar</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C9" t="inlineStr">
         <is>
           <t>Stalk of Scallions</t>
         </is>
@@ -1535,20 +1511,20 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="13" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="C1" s="13" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>Ingredient</t>
         </is>

</xml_diff>

<commit_message>
navbar to add cart icon and editing some css
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="damien" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="yc" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="User123" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -66,6 +67,9 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -87,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -114,6 +118,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1694,4 +1699,40 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="14" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="14" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="C1" s="14" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
confirmation done, left code clean up, enable otp and find out why tf i cannot redirect to homepage when clicking add-to-cart
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5250" yWindow="5505" windowWidth="38640" windowHeight="15435" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="damien" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="yc" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="User123" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="yc" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="User123" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="damien" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -22,7 +22,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -68,6 +68,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -91,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -110,15 +115,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,18 +490,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BY32"/>
+  <dimension ref="A1:CG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BU13" sqref="BU13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16.109375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="10.5546875" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="9.44140625" customWidth="1" min="22" max="22"/>
+    <col width="16.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.28515625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="10.5703125" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="9.42578125" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -884,6 +890,46 @@
           <t>Canned Tomatoes</t>
         </is>
       </c>
+      <c r="BZ1" t="inlineStr">
+        <is>
+          <t>Mushrooms</t>
+        </is>
+      </c>
+      <c r="CA1" t="inlineStr">
+        <is>
+          <t>Medium-sized Onion</t>
+        </is>
+      </c>
+      <c r="CB1" t="inlineStr">
+        <is>
+          <t>Teaspoon Mixed Herbs</t>
+        </is>
+      </c>
+      <c r="CC1" t="inlineStr">
+        <is>
+          <t>Garlic Clove</t>
+        </is>
+      </c>
+      <c r="CD1" t="inlineStr">
+        <is>
+          <t>Medium Ripe Tomatoes</t>
+        </is>
+      </c>
+      <c r="CE1" t="inlineStr">
+        <is>
+          <t>Tablespoon Cooking Oil</t>
+        </is>
+      </c>
+      <c r="CF1" t="inlineStr">
+        <is>
+          <t>Teaspoon Salt</t>
+        </is>
+      </c>
+      <c r="CG1" t="inlineStr">
+        <is>
+          <t>Pinch Sugar</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -916,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="K2" t="n">
         <v>100</v>
@@ -958,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="Y2" t="n">
         <v>150</v>
@@ -1119,6 +1165,30 @@
       <c r="BY2" t="n">
         <v>400</v>
       </c>
+      <c r="BZ2" t="n">
+        <v>250</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>700</v>
+      </c>
+      <c r="CB2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>10</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>500</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>132</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>500</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1126,233 +1196,257 @@
           <t>Price</t>
         </is>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <v>2.85</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="C3" s="12" t="n">
         <v>2.14</v>
       </c>
-      <c r="D3" s="11" t="n">
+      <c r="D3" s="12" t="n">
         <v>2.42</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="12" t="n">
         <v>1.8</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" s="12" t="n">
         <v>3.97</v>
       </c>
-      <c r="G3" s="11" t="n">
+      <c r="G3" s="12" t="n">
         <v>1.82</v>
       </c>
-      <c r="H3" s="11" t="n">
+      <c r="H3" s="12" t="n">
         <v>5.5</v>
       </c>
-      <c r="I3" s="11" t="n">
+      <c r="I3" s="12" t="n">
         <v>0.96</v>
       </c>
-      <c r="J3" s="11" t="n">
+      <c r="J3" s="12" t="n">
         <v>2.98</v>
       </c>
-      <c r="K3" s="11" t="n">
+      <c r="K3" s="12" t="n">
         <v>1.21</v>
       </c>
-      <c r="L3" s="11" t="n">
+      <c r="L3" s="12" t="n">
         <v>1.52</v>
       </c>
-      <c r="M3" s="11" t="n">
+      <c r="M3" s="12" t="n">
         <v>2.11</v>
       </c>
-      <c r="N3" s="11" t="n">
+      <c r="N3" s="12" t="n">
         <v>6.72</v>
       </c>
-      <c r="O3" s="11" t="n">
+      <c r="O3" s="12" t="n">
         <v>1.98</v>
       </c>
-      <c r="P3" s="11" t="n">
+      <c r="P3" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q3" s="11" t="n">
+      <c r="Q3" s="12" t="n">
         <v>8.5</v>
       </c>
-      <c r="R3" s="11" t="n">
+      <c r="R3" s="12" t="n">
         <v>6.45</v>
       </c>
-      <c r="S3" s="11" t="n">
+      <c r="S3" s="12" t="n">
         <v>2.21</v>
       </c>
-      <c r="T3" s="11" t="n">
+      <c r="T3" s="12" t="n">
         <v>5.85</v>
       </c>
-      <c r="U3" s="11" t="n">
+      <c r="U3" s="12" t="n">
         <v>0.46</v>
       </c>
-      <c r="V3" s="11" t="n">
+      <c r="V3" s="12" t="n">
         <v>5.95</v>
       </c>
-      <c r="W3" s="11" t="n">
+      <c r="W3" s="12" t="n">
         <v>3.82</v>
       </c>
-      <c r="X3" s="11" t="n">
+      <c r="X3" s="12" t="n">
         <v>2.98</v>
       </c>
-      <c r="Y3" s="11" t="n">
+      <c r="Y3" s="12" t="n">
         <v>4.8</v>
       </c>
-      <c r="Z3" s="11" t="n">
+      <c r="Z3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="AA3" s="11" t="n">
+      <c r="AA3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="AB3" s="11" t="n">
+      <c r="AB3" s="12" t="n">
         <v>3.75</v>
       </c>
-      <c r="AC3" s="11" t="n">
+      <c r="AC3" s="12" t="n">
         <v>1.8</v>
       </c>
-      <c r="AD3" s="11" t="n">
+      <c r="AD3" s="12" t="n">
         <v>2.22</v>
       </c>
-      <c r="AE3" s="11" t="n">
+      <c r="AE3" s="12" t="n">
         <v>9.85</v>
       </c>
-      <c r="AF3" s="11" t="n">
+      <c r="AF3" s="12" t="n">
         <v>1.99</v>
       </c>
-      <c r="AG3" s="11" t="n">
+      <c r="AG3" s="12" t="n">
         <v>1.37</v>
       </c>
-      <c r="AH3" s="11" t="n">
+      <c r="AH3" s="12" t="n">
         <v>1.12</v>
       </c>
-      <c r="AI3" s="11" t="n">
+      <c r="AI3" s="12" t="n">
         <v>1.62</v>
       </c>
-      <c r="AJ3" s="11" t="n">
+      <c r="AJ3" s="12" t="n">
         <v>0.86</v>
       </c>
-      <c r="AK3" s="11" t="n">
+      <c r="AK3" s="12" t="n">
         <v>3.65</v>
       </c>
-      <c r="AL3" s="11" t="n">
+      <c r="AL3" s="12" t="n">
         <v>3.17</v>
       </c>
-      <c r="AM3" s="11" t="n">
+      <c r="AM3" s="12" t="n">
         <v>5.98</v>
       </c>
-      <c r="AN3" s="11" t="n">
+      <c r="AN3" s="12" t="n">
         <v>4.19</v>
       </c>
-      <c r="AO3" s="11" t="n">
+      <c r="AO3" s="12" t="n">
         <v>5.66</v>
       </c>
-      <c r="AP3" s="11" t="n">
+      <c r="AP3" s="12" t="n">
         <v>3.14</v>
       </c>
-      <c r="AQ3" s="11" t="n">
+      <c r="AQ3" s="12" t="n">
         <v>7.95</v>
       </c>
-      <c r="AR3" s="11" t="n">
+      <c r="AR3" s="12" t="n">
         <v>4.5</v>
       </c>
-      <c r="AS3" s="11" t="n">
+      <c r="AS3" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="AT3" s="11" t="n">
+      <c r="AT3" s="12" t="n">
         <v>7.9</v>
       </c>
-      <c r="AU3" s="11" t="n">
+      <c r="AU3" s="12" t="n">
         <v>4.34</v>
       </c>
-      <c r="AV3" s="11" t="n">
+      <c r="AV3" s="12" t="n">
         <v>3.85</v>
       </c>
-      <c r="AW3" s="11" t="n">
+      <c r="AW3" s="12" t="n">
         <v>0.14</v>
       </c>
-      <c r="AX3" s="11" t="n">
+      <c r="AX3" s="12" t="n">
         <v>3.7</v>
       </c>
-      <c r="AY3" s="11" t="n">
+      <c r="AY3" s="12" t="n">
         <v>2.32</v>
       </c>
-      <c r="AZ3" s="11" t="n">
+      <c r="AZ3" s="12" t="n">
         <v>1.98</v>
       </c>
-      <c r="BA3" s="11" t="n">
+      <c r="BA3" s="12" t="n">
         <v>3.02</v>
       </c>
-      <c r="BB3" s="11" t="n">
+      <c r="BB3" s="12" t="n">
         <v>6.5</v>
       </c>
-      <c r="BC3" s="11" t="n">
+      <c r="BC3" s="12" t="n">
         <v>1.4</v>
       </c>
-      <c r="BD3" s="11" t="n">
+      <c r="BD3" s="12" t="n">
         <v>3.95</v>
       </c>
-      <c r="BE3" s="11" t="n">
+      <c r="BE3" s="12" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="BF3" s="11" t="n">
+      <c r="BF3" s="12" t="n">
         <v>9.9</v>
       </c>
-      <c r="BG3" s="11" t="n">
+      <c r="BG3" s="12" t="n">
         <v>1.38</v>
       </c>
-      <c r="BH3" s="11" t="n">
+      <c r="BH3" s="12" t="n">
         <v>1.15</v>
       </c>
-      <c r="BI3" s="11" t="n">
+      <c r="BI3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="BJ3" s="11" t="n">
+      <c r="BJ3" s="12" t="n">
         <v>11.91</v>
       </c>
-      <c r="BK3" s="11" t="n">
+      <c r="BK3" s="12" t="n">
         <v>5.98</v>
       </c>
-      <c r="BL3" s="11" t="n">
+      <c r="BL3" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="BM3" s="11" t="n">
+      <c r="BM3" s="12" t="n">
         <v>2.55</v>
       </c>
-      <c r="BN3" s="11" t="n">
+      <c r="BN3" s="12" t="n">
         <v>7.65</v>
       </c>
-      <c r="BO3" s="11" t="n">
+      <c r="BO3" s="12" t="n">
         <v>1.61</v>
       </c>
-      <c r="BP3" s="11" t="n">
+      <c r="BP3" s="12" t="n">
         <v>2.14</v>
       </c>
-      <c r="BQ3" s="11" t="n">
+      <c r="BQ3" s="12" t="n">
         <v>1.8</v>
       </c>
-      <c r="BR3" s="11" t="n">
+      <c r="BR3" s="12" t="n">
         <v>2.22</v>
       </c>
-      <c r="BS3" s="12" t="n">
+      <c r="BS3" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="BT3" s="11" t="n">
+      <c r="BT3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="BU3" s="11" t="n">
+      <c r="BU3" s="12" t="n">
         <v>1.82</v>
       </c>
-      <c r="BV3" s="11" t="n">
+      <c r="BV3" s="12" t="n">
         <v>6.72</v>
       </c>
-      <c r="BW3" s="11" t="n">
+      <c r="BW3" s="12" t="n">
         <v>1.98</v>
       </c>
-      <c r="BX3" s="11" t="n">
+      <c r="BX3" s="12" t="n">
         <v>1.52</v>
       </c>
-      <c r="BY3" s="11" t="n">
+      <c r="BY3" s="12" t="n">
         <v>2.85</v>
+      </c>
+      <c r="BZ3" s="12" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="CA3" s="12" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="CB3" s="12" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="CC3" s="12" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="CD3" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="CE3" s="12" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="CF3" s="12" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="CG3" s="12" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="5">
@@ -1368,7 +1462,7 @@
       <c r="AY7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n"/>
+      <c r="A8" s="14" t="n"/>
       <c r="AY8" s="2" t="n"/>
     </row>
     <row r="9">
@@ -1463,29 +1557,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="15.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>Ingredient</t>
         </is>
@@ -1493,131 +1584,40 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>37.5</v>
+        <v>30000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Carrot</t>
+          <t>Canned Tomatoes</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>8505</v>
+        <v>200</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Baby Corn</t>
+          <t>Canned Tomatoes</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>3000</v>
+        <v>150</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mushrooms</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Capsicum</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>75</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Tablespoon Unsalted Butter</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>112.5</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Garlic Cloves</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" t="n">
-        <v>300</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Slices of Bacon</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Tomato</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>75</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Onion</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Avocado</t>
+          <t>Dried Pasta</t>
         </is>
       </c>
     </row>
@@ -1627,81 +1627,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Ingredient</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>30000</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Canned Tomatoes</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>200</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Canned Tomatoes</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>150</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Dried Pasta</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1716,19 +1641,81 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="14" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="C1" s="14" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="15" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="15" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="C1" s="15" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Garlic Cloves</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Teaspoon Ginger</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
code clean up, re-enabled otp, only Tomato Pasta, Vegetable Stir Fry and Tomato Eggs work for add to cart, the rest of the ingredients i cannot be arsed to add :^)
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -1668,7 +1668,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1698,11 +1698,11 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Garlic Cloves</t>
+          <t>Capsicum</t>
         </is>
       </c>
     </row>
@@ -1715,7 +1715,46 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Tablespoon Vegetable Oil</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Garlic Cloves</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Teaspoon Ginger</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Chicken Stock</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testing shopping cart and editing otp css
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -8,8 +8,7 @@
   <sheets>
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="yc" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="User123" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="damien" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="damien" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1632,42 +1631,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Ingredient</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
changed createRecipe form 'skill' part to have radio button
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -7,8 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="yc" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="damien" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="damien" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="yc" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1556,26 +1556,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="15" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="15" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="15" t="inlineStr">
         <is>
           <t>Ingredient</t>
         </is>
@@ -1583,40 +1583,66 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>30000</v>
+        <v>0.25</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Canned Tomatoes</t>
+          <t>Capsicum</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>200</v>
+        <v>0.5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Canned Tomatoes</t>
+          <t>Tablespoon Vegetable Oil</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>150</v>
+        <v>0.75</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dried Pasta</t>
+          <t>Garlic Cloves</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Teaspoon Ginger</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Chicken Stock</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1658,66 +1684,27 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.25</v>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Capsicum</t>
+          <t>Medium Ripe Tomatoes</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.5</v>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tablespoon Vegetable Oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Garlic Cloves</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Teaspoon Ginger</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>14.79</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Chicken Stock</t>
+          <t>Eggs</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed title for view_recipes.html
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -1658,7 +1658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1706,6 +1706,32 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>Eggs</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Quinoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>200</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Canned Tomatoes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
editing already submit link
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -9,7 +9,6 @@
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="damien" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="yc" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="User123" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1683,66 +1682,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="9" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>Ingredient</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>200</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Canned Tomatoes</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>75</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Dried Pasta</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated all those cmi for display (sorry)
</commit_message>
<xml_diff>
--- a/website/Cart.xlsx
+++ b/website/Cart.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Prices" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="damien" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="yc" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="yeechingtann@gmail.com" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1645,7 +1646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -1670,16 +1671,39 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B2" t="n">
-        <v>22</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Eggs</t>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="13" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="13" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="C1" s="13" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
         </is>
       </c>
     </row>

</xml_diff>